<commit_message>
Updated the L1Menu_Collisions2024_v1_3_0 PS table according to https://its.cern.ch/jira/browse/CMSLITDPG-1318
</commit_message>
<xml_diff>
--- a/official/L1Menu_Collisions2024_v1_3_0/PrescaleTable/L1Menu_Collisions2024_v1_3_0.xlsx
+++ b/official/L1Menu_Collisions2024_v1_3_0/PrescaleTable/L1Menu_Collisions2024_v1_3_0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonar\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9116BE06-108F-49DC-BB98-AAE344E281D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6989D5CA-3344-4787-B40E-652E2D90FB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1671,8 +1671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A338" workbookViewId="0">
-      <selection activeCell="K361" sqref="K361"/>
+    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="T210" sqref="T210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14886,28 +14886,28 @@
         <v>0</v>
       </c>
       <c r="D204">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E204">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F204">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G204">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H204">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I204">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J204">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K204">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L204">
         <v>1</v>
@@ -14934,10 +14934,10 @@
         <v>0</v>
       </c>
       <c r="T204">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U204">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="205" spans="1:21" x14ac:dyDescent="0.3">
@@ -15536,58 +15536,58 @@
         <v>0</v>
       </c>
       <c r="D214">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E214">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F214">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G214">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H214">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I214">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J214">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K214">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L214">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M214">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N214">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O214">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P214">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q214">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R214">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S214">
         <v>0</v>
       </c>
       <c r="T214">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U214">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="215" spans="1:21" x14ac:dyDescent="0.3">

</xml_diff>